<commit_message>
Deployed 190a5db with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/eDNA qPCR/example output/Results_Blanks.xlsx
+++ b/eDNA qPCR/example output/Results_Blanks.xlsx
@@ -1,21 +1,147 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BoxDrive\Box\Science\Fisheries\github\resources\docs\eDNA qPCR\example output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37158E6D-4E41-4F0A-8727-4AE33242C2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-28920" yWindow="-915" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>Mean Ct</t>
+  </si>
+  <si>
+    <t>Number of Replicates</t>
+  </si>
+  <si>
+    <t>Mean Copy Number</t>
+  </si>
+  <si>
+    <t>Mean Copy Number Normalized</t>
+  </si>
+  <si>
+    <t>Detection</t>
+  </si>
+  <si>
+    <t>2024-01-17 DI Blank #1</t>
+  </si>
+  <si>
+    <t>Absent</t>
+  </si>
+  <si>
+    <t>2024-01-17 DI Blank #2</t>
+  </si>
+  <si>
+    <t>Present</t>
+  </si>
+  <si>
+    <t>2024-01-18 DI Blank #1</t>
+  </si>
+  <si>
+    <t>2024-01-18 Tap Blank #1</t>
+  </si>
+  <si>
+    <t>2024-01-24 DI Blank #1</t>
+  </si>
+  <si>
+    <t>2024-01-24 DI Blank #2</t>
+  </si>
+  <si>
+    <t>2024-01-26 Tap Blank #1</t>
+  </si>
+  <si>
+    <t>2024-01-26 Tap Blank #2</t>
+  </si>
+  <si>
+    <t>2024-02-06 Tap Blank #1</t>
+  </si>
+  <si>
+    <t>2024-02-06 Tap Blank #2</t>
+  </si>
+  <si>
+    <t>2024-02-07 Tap Blank #1</t>
+  </si>
+  <si>
+    <t>2024-02-07 Tap Blank #2</t>
+  </si>
+  <si>
+    <t>2024-02-21 Tap Blank #1</t>
+  </si>
+  <si>
+    <t>2024-02-21 Tap Blank #2</t>
+  </si>
+  <si>
+    <t>2024-03-13 Tap Blank #1</t>
+  </si>
+  <si>
+    <t>2024-03-13 Tap Blank #2</t>
+  </si>
+  <si>
+    <t>2024-03-18 Tap Blank #1</t>
+  </si>
+  <si>
+    <t>2024-03-18 Tap Blank #2</t>
+  </si>
+  <si>
+    <t>2024-03-19 Tap Blank #1</t>
+  </si>
+  <si>
+    <t>2024-03-19 Tap Blank #2</t>
+  </si>
+  <si>
+    <t>2024-03-22 Tap Blank #1</t>
+  </si>
+  <si>
+    <t>2024-03-22 Tap Blank #2</t>
+  </si>
+  <si>
+    <t>2024-05-28 Field Blank #1</t>
+  </si>
+  <si>
+    <t>2024-05-28 Field Blank #2</t>
+  </si>
+  <si>
+    <t>2024-05-28 Lab Blank #1</t>
+  </si>
+  <si>
+    <t>2024-05-28 Lab Blank #2</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +189,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -107,7 +241,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -141,6 +275,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -175,9 +310,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -350,68 +486,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Sample</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Mean Ct</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Number of Replicates</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Mean Copy Number</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Mean Copy Number Normalized</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Detection</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2024-01-17 DI Blank #1</t>
-        </is>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Absent</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2024-01-17 DI Blank #2</t>
-        </is>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>32.52</v>
+        <v>32.520000000000003</v>
       </c>
       <c r="C3">
         <v>6</v>
@@ -422,17 +550,13 @@
       <c r="E3">
         <v>1.68</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Present</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2024-01-18 DI Blank #1</t>
-        </is>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
       </c>
       <c r="B4">
         <v>38.08</v>
@@ -446,17 +570,13 @@
       <c r="E4">
         <v>0.32</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Present</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2024-01-18 Tap Blank #1</t>
-        </is>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
       </c>
       <c r="B5">
         <v>36.99</v>
@@ -470,17 +590,13 @@
       <c r="E5">
         <v>0.51</v>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Present</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2024-01-24 DI Blank #1</t>
-        </is>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
       </c>
       <c r="B6">
         <v>36.46</v>
@@ -494,47 +610,35 @@
       <c r="E6">
         <v>0.63</v>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Present</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2024-01-24 DI Blank #2</t>
-        </is>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Absent</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2024-01-26 Tap Blank #1</t>
-        </is>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Absent</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2024-01-26 Tap Blank #2</t>
-        </is>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
       </c>
       <c r="B9">
         <v>37.82</v>
@@ -548,17 +652,13 @@
       <c r="E9">
         <v>0.36</v>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Present</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2024-02-06 Tap Blank #1</t>
-        </is>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
       </c>
       <c r="B10">
         <v>36.33</v>
@@ -572,17 +672,13 @@
       <c r="E10">
         <v>0.66</v>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Present</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2024-02-06 Tap Blank #2</t>
-        </is>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>17</v>
       </c>
       <c r="B11">
         <v>34.14</v>
@@ -596,50 +692,38 @@
       <c r="E11">
         <v>1.22</v>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Present</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2024-02-07 Tap Blank #1</t>
-        </is>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>18</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Absent</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2024-02-07 Tap Blank #2</t>
-        </is>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>19</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Absent</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2024-02-21 Tap Blank #1</t>
-        </is>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>20</v>
       </c>
       <c r="B14">
-        <v>39.34</v>
+        <v>39.340000000000003</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -650,62 +734,46 @@
       <c r="E14">
         <v>0.16</v>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Present</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2024-02-21 Tap Blank #2</t>
-        </is>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>21</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Absent</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2024-03-13 Tap Blank #1</t>
-        </is>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>22</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Absent</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2024-03-13 Tap Blank #2</t>
-        </is>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>23</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Absent</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2024-03-18 Tap Blank #1</t>
-        </is>
+      <c r="F17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>24</v>
       </c>
       <c r="B18">
         <v>37.42</v>
@@ -719,62 +787,46 @@
       <c r="E18">
         <v>0.43</v>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Present</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>2024-03-18 Tap Blank #2</t>
-        </is>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>25</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Absent</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>2024-03-19 Tap Blank #1</t>
-        </is>
+      <c r="F19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>26</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Absent</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>2024-03-19 Tap Blank #2</t>
-        </is>
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>27</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Absent</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>2024-03-22 Tap Blank #1</t>
-        </is>
+      <c r="F21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>28</v>
       </c>
       <c r="B22">
         <v>38.42</v>
@@ -788,32 +840,24 @@
       <c r="E22">
         <v>0.27</v>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Present</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>2024-03-22 Tap Blank #2</t>
-        </is>
+      <c r="F22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>29</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Absent</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>2024-05-28 Field Blank #1</t>
-        </is>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>30</v>
       </c>
       <c r="B24">
         <v>36.94</v>
@@ -827,32 +871,24 @@
       <c r="E24">
         <v>0.52</v>
       </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Present</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>2024-05-28 Field Blank #2</t>
-        </is>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>31</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Absent</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>2024-05-28 Lab Blank #1</t>
-        </is>
+      <c r="F25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>32</v>
       </c>
       <c r="B26">
         <v>38.65</v>
@@ -866,25 +902,19 @@
       <c r="E26">
         <v>0.24</v>
       </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Present</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>2024-05-28 Lab Blank #2</t>
-        </is>
+      <c r="F26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>33</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Absent</t>
-        </is>
+      <c r="F27" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deployed 465f8d8 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/eDNA qPCR/example output/Results_Blanks.xlsx
+++ b/eDNA qPCR/example output/Results_Blanks.xlsx
@@ -1,147 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BoxDrive\Box\Science\Fisheries\github\resources\docs\eDNA qPCR\example output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37158E6D-4E41-4F0A-8727-4AE33242C2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-915" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
-  <si>
-    <t>Sample</t>
-  </si>
-  <si>
-    <t>Mean Ct</t>
-  </si>
-  <si>
-    <t>Number of Replicates</t>
-  </si>
-  <si>
-    <t>Mean Copy Number</t>
-  </si>
-  <si>
-    <t>Mean Copy Number Normalized</t>
-  </si>
-  <si>
-    <t>Detection</t>
-  </si>
-  <si>
-    <t>2024-01-17 DI Blank #1</t>
-  </si>
-  <si>
-    <t>Absent</t>
-  </si>
-  <si>
-    <t>2024-01-17 DI Blank #2</t>
-  </si>
-  <si>
-    <t>Present</t>
-  </si>
-  <si>
-    <t>2024-01-18 DI Blank #1</t>
-  </si>
-  <si>
-    <t>2024-01-18 Tap Blank #1</t>
-  </si>
-  <si>
-    <t>2024-01-24 DI Blank #1</t>
-  </si>
-  <si>
-    <t>2024-01-24 DI Blank #2</t>
-  </si>
-  <si>
-    <t>2024-01-26 Tap Blank #1</t>
-  </si>
-  <si>
-    <t>2024-01-26 Tap Blank #2</t>
-  </si>
-  <si>
-    <t>2024-02-06 Tap Blank #1</t>
-  </si>
-  <si>
-    <t>2024-02-06 Tap Blank #2</t>
-  </si>
-  <si>
-    <t>2024-02-07 Tap Blank #1</t>
-  </si>
-  <si>
-    <t>2024-02-07 Tap Blank #2</t>
-  </si>
-  <si>
-    <t>2024-02-21 Tap Blank #1</t>
-  </si>
-  <si>
-    <t>2024-02-21 Tap Blank #2</t>
-  </si>
-  <si>
-    <t>2024-03-13 Tap Blank #1</t>
-  </si>
-  <si>
-    <t>2024-03-13 Tap Blank #2</t>
-  </si>
-  <si>
-    <t>2024-03-18 Tap Blank #1</t>
-  </si>
-  <si>
-    <t>2024-03-18 Tap Blank #2</t>
-  </si>
-  <si>
-    <t>2024-03-19 Tap Blank #1</t>
-  </si>
-  <si>
-    <t>2024-03-19 Tap Blank #2</t>
-  </si>
-  <si>
-    <t>2024-03-22 Tap Blank #1</t>
-  </si>
-  <si>
-    <t>2024-03-22 Tap Blank #2</t>
-  </si>
-  <si>
-    <t>2024-05-28 Field Blank #1</t>
-  </si>
-  <si>
-    <t>2024-05-28 Field Blank #2</t>
-  </si>
-  <si>
-    <t>2024-05-28 Lab Blank #1</t>
-  </si>
-  <si>
-    <t>2024-05-28 Lab Blank #2</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,21 +63,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -241,7 +107,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -275,7 +141,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -310,10 +175,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -486,60 +350,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sample</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Mean Ct</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Number of Replicates</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Mean Copy Number</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Mean Copy Number Normalized</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Detection</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2024-01-17 DI Blank #1</t>
+        </is>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-01-17 DI Blank #2</t>
+        </is>
       </c>
       <c r="B3">
-        <v>32.520000000000003</v>
+        <v>32.52</v>
       </c>
       <c r="C3">
         <v>6</v>
@@ -550,13 +422,17 @@
       <c r="E3">
         <v>1.68</v>
       </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>10</v>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-01-18 DI Blank #1</t>
+        </is>
       </c>
       <c r="B4">
         <v>38.08</v>
@@ -570,13 +446,17 @@
       <c r="E4">
         <v>0.32</v>
       </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-01-18 Tap Blank #1</t>
+        </is>
       </c>
       <c r="B5">
         <v>36.99</v>
@@ -590,13 +470,17 @@
       <c r="E5">
         <v>0.51</v>
       </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-01-24 DI Blank #1</t>
+        </is>
       </c>
       <c r="B6">
         <v>36.46</v>
@@ -610,35 +494,47 @@
       <c r="E6">
         <v>0.63</v>
       </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>13</v>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-01-24 DI Blank #2</t>
+        </is>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>14</v>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-01-26 Tap Blank #1</t>
+        </is>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="F8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>15</v>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-01-26 Tap Blank #2</t>
+        </is>
       </c>
       <c r="B9">
         <v>37.82</v>
@@ -652,13 +548,17 @@
       <c r="E9">
         <v>0.36</v>
       </c>
-      <c r="F9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>16</v>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-02-06 Tap Blank #1</t>
+        </is>
       </c>
       <c r="B10">
         <v>36.33</v>
@@ -672,13 +572,17 @@
       <c r="E10">
         <v>0.66</v>
       </c>
-      <c r="F10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>17</v>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-02-06 Tap Blank #2</t>
+        </is>
       </c>
       <c r="B11">
         <v>34.14</v>
@@ -692,38 +596,50 @@
       <c r="E11">
         <v>1.22</v>
       </c>
-      <c r="F11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>18</v>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-02-07 Tap Blank #1</t>
+        </is>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
-      <c r="F12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>19</v>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-02-07 Tap Blank #2</t>
+        </is>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
-      <c r="F13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>20</v>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-02-21 Tap Blank #1</t>
+        </is>
       </c>
       <c r="B14">
-        <v>39.340000000000003</v>
+        <v>39.34</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -734,46 +650,62 @@
       <c r="E14">
         <v>0.16</v>
       </c>
-      <c r="F14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>21</v>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-02-21 Tap Blank #2</t>
+        </is>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
-      <c r="F15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>22</v>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-03-13 Tap Blank #1</t>
+        </is>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
-      <c r="F16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>23</v>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-03-13 Tap Blank #2</t>
+        </is>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
-      <c r="F17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>24</v>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-03-18 Tap Blank #1</t>
+        </is>
       </c>
       <c r="B18">
         <v>37.42</v>
@@ -787,46 +719,62 @@
       <c r="E18">
         <v>0.43</v>
       </c>
-      <c r="F18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>25</v>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-03-18 Tap Blank #2</t>
+        </is>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
-      <c r="F19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>26</v>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-03-19 Tap Blank #1</t>
+        </is>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
-      <c r="F20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>27</v>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-03-19 Tap Blank #2</t>
+        </is>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
-      <c r="F21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>28</v>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-03-22 Tap Blank #1</t>
+        </is>
       </c>
       <c r="B22">
         <v>38.42</v>
@@ -840,24 +788,32 @@
       <c r="E22">
         <v>0.27</v>
       </c>
-      <c r="F22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>29</v>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-03-22 Tap Blank #2</t>
+        </is>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
-      <c r="F23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>30</v>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-05-28 Field Blank #1</t>
+        </is>
       </c>
       <c r="B24">
         <v>36.94</v>
@@ -871,24 +827,32 @@
       <c r="E24">
         <v>0.52</v>
       </c>
-      <c r="F24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>31</v>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-05-28 Field Blank #2</t>
+        </is>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
-      <c r="F25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>32</v>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-05-28 Lab Blank #1</t>
+        </is>
       </c>
       <c r="B26">
         <v>38.65</v>
@@ -902,19 +866,25 @@
       <c r="E26">
         <v>0.24</v>
       </c>
-      <c r="F26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>33</v>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-05-28 Lab Blank #2</t>
+        </is>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
-      <c r="F27" t="s">
-        <v>7</v>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deployed f9907dc with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/eDNA qPCR/example output/Results_Blanks.xlsx
+++ b/eDNA qPCR/example output/Results_Blanks.xlsx
@@ -417,7 +417,7 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>47.72</v>
+        <v>47.67</v>
       </c>
       <c r="E3">
         <v>1.69</v>
@@ -465,7 +465,7 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>2.3</v>
+        <v>2.29</v>
       </c>
       <c r="E5">
         <v>0.52</v>
@@ -489,7 +489,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>3.3</v>
+        <v>3.29</v>
       </c>
       <c r="E6">
         <v>0.63</v>
@@ -567,7 +567,7 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>3.6</v>
+        <v>3.59</v>
       </c>
       <c r="E10">
         <v>0.66</v>
@@ -591,7 +591,7 @@
         <v>6</v>
       </c>
       <c r="D11">
-        <v>15.87</v>
+        <v>15.88</v>
       </c>
       <c r="E11">
         <v>1.23</v>

</xml_diff>